<commit_message>
Updated resuts, model selection, main effects and multiple comparisons
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">family</t>
   </si>
@@ -47,19 +47,16 @@
     <t xml:space="preserve">BIC</t>
   </si>
   <si>
-    <t xml:space="preserve">deviance</t>
-  </si>
-  <si>
     <t xml:space="preserve">df.residual</t>
   </si>
   <si>
-    <t xml:space="preserve">Gamma</t>
+    <t xml:space="preserve">lognormal</t>
   </si>
   <si>
     <t xml:space="preserve">log</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_accel ~ habitat_type * season + (1 | animal_id)</t>
+    <t xml:space="preserve">mean_accel ~ habitat_type * season + (1 | animal_id) + ar1(season + 0 | animal_id) + ar1(habitat_type + 0 | animal_id)</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -443,34 +440,31 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" t="n">
         <v>16824</v>
       </c>
       <c r="F2" t="n">
-        <v>0.662856216238388</v>
+        <v>0.367886140934635</v>
       </c>
       <c r="G2" t="n">
-        <v>4536.19637538216</v>
+        <v>3453.37736771149</v>
       </c>
       <c r="H2" t="n">
-        <v>-9032.39275076432</v>
+        <v>-6858.75473542298</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -479,94 +473,85 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-8877.78151641667</v>
+        <v>-6673.2212542058</v>
       </c>
       <c r="L2" t="n">
-        <v>7916.95827747725</v>
-      </c>
-      <c r="M2" t="n">
-        <v>16804</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="n">
-        <v>17133</v>
+        <v>16824</v>
       </c>
       <c r="F3" t="n">
-        <v>0.668656623552693</v>
+        <v>0.373938160111812</v>
       </c>
       <c r="G3" t="n">
-        <v>4275.30267579662</v>
+        <v>3280.52269517336</v>
       </c>
       <c r="H3" t="n">
-        <v>-8538.60535159325</v>
+        <v>-6549.04539034673</v>
       </c>
       <c r="I3" t="n">
-        <v>493.787399171073</v>
+        <v>309.709345076252</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000596250358707656</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000559075189607128</v>
       </c>
       <c r="K3" t="n">
-        <v>-8492.11278134925</v>
+        <v>-6502.66202004243</v>
       </c>
       <c r="L3" t="n">
-        <v>8213.46993103883</v>
-      </c>
-      <c r="M3" t="n">
-        <v>17127</v>
+        <v>16818</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
       </c>
       <c r="E4" t="n">
         <v>16824</v>
       </c>
       <c r="F4" t="n">
-        <v>0.792150335371764</v>
+        <v>0.375750086752719</v>
       </c>
       <c r="G4" t="n">
-        <v>1026.69043939897</v>
+        <v>2140.6878653588</v>
       </c>
       <c r="H4" t="n">
-        <v>-2039.38087879795</v>
+        <v>-4267.3757307176</v>
       </c>
       <c r="I4" t="n">
-        <v>6993.01187196637</v>
+        <v>2591.37900470538</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>-1985.26694677627</v>
+        <v>-4213.26179869592</v>
       </c>
       <c r="L4" t="n">
-        <v>11613.5269619364</v>
-      </c>
-      <c r="M4" t="n">
         <v>16817</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated  main and ind effects, and model selection outputs and mulitple comparisions
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">family</t>
   </si>
@@ -56,16 +56,43 @@
     <t xml:space="preserve">log</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_accel ~ habitat_type * season + (1 | animal_id) + ar1(season + 0 | animal_id) + ar1(habitat_type + 0 | animal_id)</t>
+    <t xml:space="preserve">mean_accel ~ habitat_type * season * day_night + (1 | animal_id) + ar1(season + 0 | animal_id)</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
+    <t xml:space="preserve">mean_accel ~ season + day_night + (1 | animal_id) + season:day_night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_accel ~ habitat_type + season + (1 | animal_id) + habitat_type:season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m4</t>
+  </si>
+  <si>
     <t xml:space="preserve">mean_accel ~ season + (1 | animal_id)</t>
   </si>
   <si>
     <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_accel ~ habitat_type + day_night + (1 | animal_id) + habitat_type:day_night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_accel ~ day_night + (1 | animal_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3</t>
   </si>
   <si>
     <t xml:space="preserve">mean_accel ~ habitat_type + (1 | animal_id)</t>
@@ -455,16 +482,16 @@
         <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>16824</v>
+        <v>18539</v>
       </c>
       <c r="F2" t="n">
-        <v>0.367886140934635</v>
+        <v>0.368452446462205</v>
       </c>
       <c r="G2" t="n">
-        <v>3453.37736771149</v>
+        <v>4002.95079718084</v>
       </c>
       <c r="H2" t="n">
-        <v>-6858.75473542298</v>
+        <v>-7869.90159436169</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -473,10 +500,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-6673.2212542058</v>
+        <v>-7337.62262514587</v>
       </c>
       <c r="L2" t="n">
-        <v>16800</v>
+        <v>18471</v>
       </c>
     </row>
     <row r="3">
@@ -493,28 +520,28 @@
         <v>17</v>
       </c>
       <c r="E3" t="n">
-        <v>16824</v>
+        <v>18539</v>
       </c>
       <c r="F3" t="n">
-        <v>0.373938160111812</v>
+        <v>0.376870079516635</v>
       </c>
       <c r="G3" t="n">
-        <v>3280.52269517336</v>
+        <v>3729.37131394347</v>
       </c>
       <c r="H3" t="n">
-        <v>-6549.04539034673</v>
+        <v>-7422.74262788694</v>
       </c>
       <c r="I3" t="n">
-        <v>309.709345076252</v>
+        <v>447.158966474748</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000559075189607128</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000795543924150648</v>
       </c>
       <c r="K3" t="n">
-        <v>-6502.66202004243</v>
+        <v>-7281.84525368275</v>
       </c>
       <c r="L3" t="n">
-        <v>16818</v>
+        <v>18521</v>
       </c>
     </row>
     <row r="4">
@@ -531,28 +558,218 @@
         <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>16824</v>
+        <v>18539</v>
       </c>
       <c r="F4" t="n">
-        <v>0.375750086752719</v>
+        <v>0.383810591934266</v>
       </c>
       <c r="G4" t="n">
-        <v>2140.6878653588</v>
+        <v>3279.01963096275</v>
       </c>
       <c r="H4" t="n">
-        <v>-4267.3757307176</v>
+        <v>-6518.0392619255</v>
       </c>
       <c r="I4" t="n">
-        <v>2591.37900470538</v>
+        <v>1351.86233243619</v>
       </c>
       <c r="J4" t="n">
+        <v>2.79784960010847e-294</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-6361.48662392085</v>
+      </c>
+      <c r="L4" t="n">
+        <v>18519</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18539</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.387027149613895</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3182.15379064369</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-6352.30758128738</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1517.59401307431</v>
+      </c>
+      <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="n">
-        <v>-4213.26179869592</v>
-      </c>
-      <c r="L4" t="n">
-        <v>16817</v>
+      <c r="K5" t="n">
+        <v>-6305.34178988598</v>
+      </c>
+      <c r="L5" t="n">
+        <v>18533</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="n">
+        <v>18539</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.381863469281159</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2460.89752126732</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-4877.79504253465</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2992.10655182704</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-4705.58714072953</v>
+      </c>
+      <c r="L6" t="n">
+        <v>18517</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18539</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.381863469281159</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2460.89752126732</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-4877.79504253465</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2992.10655182704</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-4705.58714072953</v>
+      </c>
+      <c r="L7" t="n">
+        <v>18517</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18539</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.387667847897727</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2286.96015148016</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-4561.92030296032</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3307.98129140137</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-4514.95451155893</v>
+      </c>
+      <c r="L8" t="n">
+        <v>18533</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18539</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.390232291554728</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1913.36153476976</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-3812.72306953952</v>
+      </c>
+      <c r="I9" t="n">
+        <v>4057.17852482217</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-3757.92964623789</v>
+      </c>
+      <c r="L9" t="n">
+        <v>18532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated lmb model outputs and effects
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
@@ -485,13 +485,13 @@
         <v>18539</v>
       </c>
       <c r="F2" t="n">
-        <v>0.368452446462205</v>
+        <v>0.368452594287898</v>
       </c>
       <c r="G2" t="n">
-        <v>4002.95079718084</v>
+        <v>4002.950797196</v>
       </c>
       <c r="H2" t="n">
-        <v>-7869.90159436169</v>
+        <v>-7869.901594392</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-7337.62262514587</v>
+        <v>-7337.62262517619</v>
       </c>
       <c r="L2" t="n">
         <v>18471</v>
@@ -532,10 +532,10 @@
         <v>-7422.74262788694</v>
       </c>
       <c r="I3" t="n">
-        <v>447.158966474748</v>
+        <v>447.158966505063</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000795543924150648</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000079554391209208</v>
       </c>
       <c r="K3" t="n">
         <v>-7281.84525368275</v>
@@ -561,22 +561,22 @@
         <v>18539</v>
       </c>
       <c r="F4" t="n">
-        <v>0.383810591934266</v>
+        <v>0.383810591931511</v>
       </c>
       <c r="G4" t="n">
-        <v>3279.01963096275</v>
+        <v>3279.01963096276</v>
       </c>
       <c r="H4" t="n">
-        <v>-6518.0392619255</v>
+        <v>-6518.03926192552</v>
       </c>
       <c r="I4" t="n">
-        <v>1351.86233243619</v>
+        <v>1351.86233246648</v>
       </c>
       <c r="J4" t="n">
-        <v>2.79784960010847e-294</v>
+        <v>2.79784955772513e-294</v>
       </c>
       <c r="K4" t="n">
-        <v>-6361.48662392085</v>
+        <v>-6361.48662392087</v>
       </c>
       <c r="L4" t="n">
         <v>18519</v>
@@ -608,7 +608,7 @@
         <v>-6352.30758128738</v>
       </c>
       <c r="I5" t="n">
-        <v>1517.59401307431</v>
+        <v>1517.59401310462</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>-4877.79504253465</v>
       </c>
       <c r="I6" t="n">
-        <v>2992.10655182704</v>
+        <v>2992.10655185736</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -684,7 +684,7 @@
         <v>-4877.79504253465</v>
       </c>
       <c r="I7" t="n">
-        <v>2992.10655182704</v>
+        <v>2992.10655185736</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>-4561.92030296032</v>
       </c>
       <c r="I8" t="n">
-        <v>3307.98129140137</v>
+        <v>3307.98129143168</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -760,7 +760,7 @@
         <v>-3812.72306953952</v>
       </c>
       <c r="I9" t="n">
-        <v>4057.17852482217</v>
+        <v>4057.17852485248</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updated lmb model selection
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_lmb.xlsx
@@ -485,13 +485,13 @@
         <v>18539</v>
       </c>
       <c r="F2" t="n">
-        <v>0.368452594287898</v>
+        <v>0.368452425033046</v>
       </c>
       <c r="G2" t="n">
-        <v>4002.950797196</v>
+        <v>4002.95079720842</v>
       </c>
       <c r="H2" t="n">
-        <v>-7869.901594392</v>
+        <v>-7869.90159441683</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-7337.62262517619</v>
+        <v>-7337.62262520102</v>
       </c>
       <c r="L2" t="n">
         <v>18471</v>
@@ -532,10 +532,10 @@
         <v>-7422.74262788694</v>
       </c>
       <c r="I3" t="n">
-        <v>447.158966505063</v>
+        <v>447.158966529893</v>
       </c>
       <c r="J3" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000079554391209208</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000795543902215357</v>
       </c>
       <c r="K3" t="n">
         <v>-7281.84525368275</v>
@@ -570,10 +570,10 @@
         <v>-6518.03926192552</v>
       </c>
       <c r="I4" t="n">
-        <v>1351.86233246648</v>
+        <v>1351.86233249131</v>
       </c>
       <c r="J4" t="n">
-        <v>2.79784955772513e-294</v>
+        <v>2.79784952298966e-294</v>
       </c>
       <c r="K4" t="n">
         <v>-6361.48662392087</v>
@@ -608,7 +608,7 @@
         <v>-6352.30758128738</v>
       </c>
       <c r="I5" t="n">
-        <v>1517.59401310462</v>
+        <v>1517.59401312945</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>-4877.79504253465</v>
       </c>
       <c r="I6" t="n">
-        <v>2992.10655185736</v>
+        <v>2992.10655188219</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -684,7 +684,7 @@
         <v>-4877.79504253465</v>
       </c>
       <c r="I7" t="n">
-        <v>2992.10655185736</v>
+        <v>2992.10655188219</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>-4561.92030296032</v>
       </c>
       <c r="I8" t="n">
-        <v>3307.98129143168</v>
+        <v>3307.98129145651</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -760,7 +760,7 @@
         <v>-3812.72306953952</v>
       </c>
       <c r="I9" t="n">
-        <v>4057.17852485248</v>
+        <v>4057.17852487731</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>

</xml_diff>